<commit_message>
flipped graph and exp 1 code
</commit_message>
<xml_diff>
--- a/lab5/1/pMOS_exp1_flipped.xlsx
+++ b/lab5/1/pMOS_exp1_flipped.xlsx
@@ -16,10 +16,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>V_G</t>
+    <t>V_PMOS</t>
   </si>
   <si>
-    <t xml:space="preserve"> I_channel0.0</t>
+    <t>I_PMOS</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v> I_channel0.0</c:v>
+                  <c:v>I_PMOS</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2448,11 +2448,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="575592064"/>
-        <c:axId val="575591488"/>
+        <c:axId val="73327744"/>
+        <c:axId val="73328320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="575592064"/>
+        <c:axId val="73327744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2462,12 +2462,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="575591488"/>
+        <c:crossAx val="73328320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="575591488"/>
+        <c:axId val="73328320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2478,7 +2478,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="575592064"/>
+        <c:crossAx val="73327744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2825,7 +2825,7 @@
   <dimension ref="A1:B301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>